<commit_message>
Update the raw data collection(sanity check, iotamotion device) plus unit correction on graph
</commit_message>
<xml_diff>
--- a/output_file/July X=20/example.xlsx
+++ b/output_file/July X=20/example.xlsx
@@ -37,31 +37,31 @@
     <t>MetalNumber</t>
   </si>
   <si>
+    <t>Control</t>
+  </si>
+  <si>
     <t>LC Steel</t>
   </si>
   <si>
+    <t>416 SS</t>
+  </si>
+  <si>
+    <t>304 SS</t>
+  </si>
+  <si>
+    <t>6061 Al</t>
+  </si>
+  <si>
+    <t>Ti Grade 5</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
     <t>Validity_Check_Value_of_Translation_Error</t>
   </si>
   <si>
     <t>Validity_Check_Value_of_Rotation_Error</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>416 SS</t>
-  </si>
-  <si>
-    <t>304 SS</t>
-  </si>
-  <si>
-    <t>6061 Al</t>
-  </si>
-  <si>
-    <t>Ti Grade 5</t>
-  </si>
-  <si>
-    <t>Copper</t>
   </si>
 </sst>
 </file>
@@ -399,10 +399,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -410,7 +410,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>2.5298811965624899E-7</v>
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>3.5964066919069565E-6</v>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>4.2655653257349922E-7</v>
@@ -452,7 +452,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>1.1292082171948406E-6</v>
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>3.6493640170996623E-6</v>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>1.9637988763980749E-6</v>
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>5.0093775271640976E-7</v>

</xml_diff>